<commit_message>
Thinking/working on this a bit...
</commit_message>
<xml_diff>
--- a/misc/2020-spring-honors-project-time-tracking.xlsx
+++ b/misc/2020-spring-honors-project-time-tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsteele/OneDrive - Madison College/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thsteele\Documents\GitHub\klask\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{A61A8A38-0C92-7B48-BF10-626A0E4571B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA712F05-C250-164C-824B-8223A0EEF6AA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94873326-B07B-4F49-B3F6-5F40D3562042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="12340" xr2:uid="{613854B7-9CDC-244D-8F0F-8C1BABD8EA08}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{613854B7-9CDC-244D-8F0F-8C1BABD8EA08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>burn-up, ionic, ????</t>
+  </si>
+  <si>
+    <t>tsteele/reduce-experiments</t>
+  </si>
+  <si>
+    <t>TypeScript playground reduce experiments, hmmm</t>
   </si>
 </sst>
 </file>
@@ -166,8 +172,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0284A285-D743-7F49-94A0-B75FE14E2D14}" name="Table1" displayName="Table1" ref="A1:F6" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F6" xr:uid="{DD7AA787-0551-B645-AC85-B255A9D04067}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0284A285-D743-7F49-94A0-B75FE14E2D14}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F8" xr:uid="{DD7AA787-0551-B645-AC85-B255A9D04067}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D9696841-FDED-7641-85B0-190B9E940920}" name="date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{189A8903-497C-734A-9F44-57AEAEC2F35F}" name="who"/>
@@ -479,19 +485,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD03E2B8-8DA1-8B4C-9364-C9C9F806DD97}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.3125" customWidth="1"/>
+    <col min="6" max="6" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -511,7 +517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>43871</v>
       </c>
@@ -532,7 +538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>43881</v>
       </c>
@@ -553,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>43892</v>
       </c>
@@ -574,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>43899</v>
       </c>
@@ -595,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>43902</v>
       </c>
@@ -614,6 +620,38 @@
       </c>
       <c r="F6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A7" s="1">
+        <v>43902</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A8" s="1">
+        <v>43903</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>